<commit_message>
Updated and moved section "Parse trees"
</commit_message>
<xml_diff>
--- a/JSEP submission/data/4. results/depths.xlsx
+++ b/JSEP submission/data/4. results/depths.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="132" windowWidth="18180" windowHeight="6912"/>
+    <workbookView xWindow="390" yWindow="135" windowWidth="18180" windowHeight="6915"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1026,11 +1026,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="361900288"/>
-        <c:axId val="361939328"/>
+        <c:axId val="304191360"/>
+        <c:axId val="304197632"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="361900288"/>
+        <c:axId val="304191360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="430"/>
@@ -1061,12 +1061,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="361939328"/>
+        <c:crossAx val="304197632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="361939328"/>
+        <c:axId val="304197632"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1079,7 +1079,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="361900288"/>
+        <c:crossAx val="304191360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1754,11 +1754,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="362220928"/>
-        <c:axId val="362223104"/>
+        <c:axId val="304208896"/>
+        <c:axId val="304358528"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="362220928"/>
+        <c:axId val="304208896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="220"/>
@@ -1801,12 +1801,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="362223104"/>
+        <c:crossAx val="304358528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="362223104"/>
+        <c:axId val="304358528"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1815,11 +1815,30 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Unique formulas</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="#,##0" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="362220928"/>
+        <c:crossAx val="304208896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2500,11 +2519,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="362246912"/>
-        <c:axId val="362248832"/>
+        <c:axId val="304374144"/>
+        <c:axId val="304376064"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="362246912"/>
+        <c:axId val="304374144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="220"/>
@@ -2535,12 +2554,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="362248832"/>
+        <c:crossAx val="304376064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="362248832"/>
+        <c:axId val="304376064"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2549,11 +2568,30 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Unique formulas</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="#,##0" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="362246912"/>
+        <c:crossAx val="304374144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2748,11 +2786,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="362270080"/>
-        <c:axId val="362350080"/>
+        <c:axId val="304385024"/>
+        <c:axId val="304411776"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="362270080"/>
+        <c:axId val="304385024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="27"/>
@@ -2791,12 +2829,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="362350080"/>
+        <c:crossAx val="304411776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="362350080"/>
+        <c:axId val="304411776"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2805,11 +2843,30 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Unique formulas</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="#,##0" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="362270080"/>
+        <c:crossAx val="304385024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3246,21 +3303,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="B22" workbookViewId="0">
+      <selection activeCell="K55" sqref="K55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.21875" customWidth="1"/>
-    <col min="11" max="11" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" customWidth="1"/>
+    <col min="11" max="11" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3286,7 +3343,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -3312,7 +3369,7 @@
         <v>7550128</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>4</v>
       </c>
@@ -3338,7 +3395,7 @@
         <v>805359</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>5</v>
       </c>
@@ -3364,7 +3421,7 @@
         <v>172532</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>6</v>
       </c>
@@ -3390,7 +3447,7 @@
         <v>20492</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>7</v>
       </c>
@@ -3416,7 +3473,7 @@
         <v>21124</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>8</v>
       </c>
@@ -3442,7 +3499,7 @@
         <v>2518</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>9</v>
       </c>
@@ -3468,7 +3525,7 @@
         <v>2303</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>10</v>
       </c>
@@ -3494,7 +3551,7 @@
         <v>1182</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>11</v>
       </c>
@@ -3520,7 +3577,7 @@
         <v>1241</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>12</v>
       </c>
@@ -3546,7 +3603,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>13</v>
       </c>
@@ -3572,7 +3629,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>14</v>
       </c>
@@ -3598,7 +3655,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>15</v>
       </c>
@@ -3624,7 +3681,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>16</v>
       </c>
@@ -3650,7 +3707,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>17</v>
       </c>
@@ -3676,7 +3733,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>18</v>
       </c>
@@ -3702,7 +3759,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>19</v>
       </c>
@@ -3728,7 +3785,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>20</v>
       </c>
@@ -3754,7 +3811,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>21</v>
       </c>
@@ -3774,7 +3831,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>22</v>
       </c>
@@ -3802,7 +3859,7 @@
         <v>3.3578295549395129E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>23</v>
       </c>
@@ -3826,7 +3883,7 @@
         <v>8576969</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>24</v>
       </c>
@@ -3846,7 +3903,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>25</v>
       </c>
@@ -3866,7 +3923,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>26</v>
       </c>
@@ -3886,7 +3943,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>27</v>
       </c>
@@ -3906,7 +3963,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>28</v>
       </c>
@@ -3926,7 +3983,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>29</v>
       </c>
@@ -3946,7 +4003,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>30</v>
       </c>
@@ -3966,7 +4023,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>31</v>
       </c>
@@ -3986,7 +4043,7 @@
         <v>3022</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>32</v>
       </c>
@@ -4006,7 +4063,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>33</v>
       </c>
@@ -4026,7 +4083,7 @@
         <v>3195</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>34</v>
       </c>
@@ -4046,7 +4103,7 @@
         <v>3054</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>35</v>
       </c>
@@ -4066,7 +4123,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>36</v>
       </c>
@@ -4086,7 +4143,7 @@
         <v>3040</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>37</v>
       </c>
@@ -4106,7 +4163,7 @@
         <v>2985</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>38</v>
       </c>
@@ -4126,7 +4183,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>39</v>
       </c>
@@ -4146,7 +4203,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>40</v>
       </c>
@@ -4166,7 +4223,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>41</v>
       </c>
@@ -4186,7 +4243,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>42</v>
       </c>
@@ -4206,7 +4263,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>43</v>
       </c>
@@ -4226,7 +4283,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>44</v>
       </c>
@@ -4246,7 +4303,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>45</v>
       </c>
@@ -4266,7 +4323,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>46</v>
       </c>
@@ -4286,7 +4343,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>47</v>
       </c>
@@ -4306,7 +4363,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>48</v>
       </c>
@@ -4326,7 +4383,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>49</v>
       </c>
@@ -4346,7 +4403,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>50</v>
       </c>
@@ -4366,7 +4423,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>51</v>
       </c>
@@ -4386,7 +4443,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>52</v>
       </c>
@@ -4406,7 +4463,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>53</v>
       </c>
@@ -4426,7 +4483,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>54</v>
       </c>
@@ -4446,7 +4503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>55</v>
       </c>
@@ -4466,7 +4523,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>56</v>
       </c>
@@ -4486,7 +4543,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>57</v>
       </c>
@@ -4506,7 +4563,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>58</v>
       </c>
@@ -4526,7 +4583,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>59</v>
       </c>
@@ -4546,7 +4603,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>60</v>
       </c>
@@ -4566,7 +4623,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>61</v>
       </c>
@@ -4586,7 +4643,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>62</v>
       </c>
@@ -4606,7 +4663,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>63</v>
       </c>
@@ -4626,7 +4683,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>64</v>
       </c>
@@ -4646,7 +4703,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>65</v>
       </c>
@@ -4666,7 +4723,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>66</v>
       </c>
@@ -4686,7 +4743,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>67</v>
       </c>
@@ -4706,7 +4763,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>68</v>
       </c>
@@ -4726,7 +4783,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>69</v>
       </c>
@@ -4746,7 +4803,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>70</v>
       </c>
@@ -4766,7 +4823,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>71</v>
       </c>
@@ -4786,7 +4843,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>72</v>
       </c>
@@ -4806,7 +4863,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>73</v>
       </c>
@@ -4826,7 +4883,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>74</v>
       </c>
@@ -4846,7 +4903,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>76</v>
       </c>
@@ -4866,7 +4923,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>77</v>
       </c>
@@ -4886,7 +4943,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>78</v>
       </c>
@@ -4906,7 +4963,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>80</v>
       </c>
@@ -4926,7 +4983,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>82</v>
       </c>
@@ -4946,7 +5003,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>84</v>
       </c>
@@ -4966,7 +5023,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>85</v>
       </c>
@@ -4986,7 +5043,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>86</v>
       </c>
@@ -5006,7 +5063,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>88</v>
       </c>
@@ -5026,7 +5083,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>90</v>
       </c>
@@ -5046,7 +5103,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>92</v>
       </c>
@@ -5066,7 +5123,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>94</v>
       </c>
@@ -5086,7 +5143,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>95</v>
       </c>
@@ -5106,7 +5163,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>96</v>
       </c>
@@ -5126,7 +5183,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>97</v>
       </c>
@@ -5146,7 +5203,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>98</v>
       </c>
@@ -5166,7 +5223,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>100</v>
       </c>
@@ -5186,7 +5243,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>102</v>
       </c>
@@ -5206,7 +5263,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>104</v>
       </c>
@@ -5226,7 +5283,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>106</v>
       </c>
@@ -5246,7 +5303,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>107</v>
       </c>
@@ -5266,7 +5323,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>108</v>
       </c>
@@ -5286,7 +5343,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>110</v>
       </c>
@@ -5306,7 +5363,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>112</v>
       </c>
@@ -5326,7 +5383,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>114</v>
       </c>
@@ -5346,7 +5403,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>115</v>
       </c>
@@ -5366,7 +5423,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>116</v>
       </c>
@@ -5380,7 +5437,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>118</v>
       </c>
@@ -5388,7 +5445,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>120</v>
       </c>
@@ -5396,7 +5453,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>121</v>
       </c>
@@ -5404,7 +5461,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>122</v>
       </c>
@@ -5412,7 +5469,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>123</v>
       </c>
@@ -5420,7 +5477,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>124</v>
       </c>
@@ -5428,7 +5485,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>125</v>
       </c>
@@ -5436,7 +5493,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>126</v>
       </c>
@@ -5444,7 +5501,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>128</v>
       </c>
@@ -5452,7 +5509,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>130</v>
       </c>
@@ -5460,7 +5517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>132</v>
       </c>
@@ -5468,7 +5525,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>134</v>
       </c>
@@ -5476,7 +5533,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>136</v>
       </c>
@@ -5484,7 +5541,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>138</v>
       </c>
@@ -5492,7 +5549,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>146</v>
       </c>
@@ -5500,7 +5557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>150</v>
       </c>
@@ -5508,7 +5565,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>155</v>
       </c>
@@ -5516,7 +5573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>156</v>
       </c>
@@ -5524,7 +5581,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>158</v>
       </c>
@@ -5532,7 +5589,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>160</v>
       </c>
@@ -5540,7 +5597,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>162</v>
       </c>
@@ -5548,7 +5605,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>164</v>
       </c>
@@ -5556,7 +5613,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>166</v>
       </c>
@@ -5564,7 +5621,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>168</v>
       </c>
@@ -5572,7 +5629,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>170</v>
       </c>
@@ -5580,7 +5637,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>178</v>
       </c>
@@ -5588,7 +5645,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>182</v>
       </c>
@@ -5596,7 +5653,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>187</v>
       </c>
@@ -5604,7 +5661,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>188</v>
       </c>
@@ -5612,7 +5669,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>192</v>
       </c>
@@ -5620,7 +5677,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>196</v>
       </c>
@@ -5628,7 +5685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>205</v>
       </c>
@@ -5636,7 +5693,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>207</v>
       </c>
@@ -5644,7 +5701,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>212</v>
       </c>
@@ -5652,7 +5709,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>214</v>
       </c>
@@ -5660,7 +5717,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>230</v>
       </c>
@@ -5668,7 +5725,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>246</v>
       </c>
@@ -5676,7 +5733,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>252</v>
       </c>
@@ -5684,7 +5741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>276</v>
       </c>
@@ -5692,7 +5749,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>280</v>
       </c>
@@ -5700,7 +5757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>296</v>
       </c>
@@ -5708,7 +5765,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>310</v>
       </c>
@@ -5716,7 +5773,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>350</v>
       </c>
@@ -5724,7 +5781,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>380</v>
       </c>
@@ -5732,7 +5789,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>404</v>
       </c>
@@ -5740,7 +5797,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>420</v>
       </c>
@@ -5748,7 +5805,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B147" s="1"/>
     </row>
   </sheetData>
@@ -5764,7 +5821,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5776,7 +5833,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>